<commit_message>
Add province and type of car
</commit_message>
<xml_diff>
--- a/Header_SAP.xlsx
+++ b/Header_SAP.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27511"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{626A343A-4A45-41EC-BAD5-A8FA4FF900F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED2E4CFB-8CA6-4C81-A589-0BE8BCD3BC54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>FileName</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>License2</t>
+  </si>
+  <si>
+    <t>Province</t>
+  </si>
+  <si>
+    <t>TypeOfCar</t>
   </si>
   <si>
     <t>WH</t>
@@ -88,13 +94,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="222"/>
     </font>
   </fonts>
   <fills count="2">
@@ -117,8 +130,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,13 +447,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -461,10 +477,10 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J1" t="s">
@@ -490,6 +506,12 @@
       </c>
       <c r="Q1" t="s">
         <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>